<commit_message>
fix order, send sms
</commit_message>
<xml_diff>
--- a/public/file/add_receivers_template.xlsx
+++ b/public/file/add_receivers_template.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\-\Desktop\degmerchant\degmerchant\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68459C84-98FF-4028-BCE3-0D179FC17282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21480" windowHeight="8340" xr2:uid="{E2FB6290-EDD7-4EFC-A51E-F89522859E38}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="21480" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Phone</t>
   </si>
@@ -48,17 +42,26 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Time1</t>
+  </si>
+  <si>
+    <t>Time2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -66,7 +69,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -100,74 +103,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -184,10 +119,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -222,7 +157,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -274,7 +209,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -468,28 +403,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943BFEF6-3D49-4FB7-B581-F7CFBC90C95E}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
+    <col min="3" max="3" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,8 +434,17 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>